<commit_message>
Update write result just one column
</commit_message>
<xml_diff>
--- a/TSP_Result.xlsx
+++ b/TSP_Result.xlsx
@@ -83,6 +83,246 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>38.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>38.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>38.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B13" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B16" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B17" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B18" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B19" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B20" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="B21" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="B22" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="B23" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="B24" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="B25" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="B26" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="B27" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="B28" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="B29" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="B30" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="B31" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>